<commit_message>
Updating a spec file
</commit_message>
<xml_diff>
--- a/public/src/modules/BulkLoadContainersFromSDF/spec/BulkLoadContainersFromSDF_ACASmap.xlsx
+++ b/public/src/modules/BulkLoadContainersFromSDF/spec/BulkLoadContainersFromSDF_ACASmap.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="-1500" yWindow="-18380" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
@@ -27,7 +27,7 @@
     <author>Samuel Meyer</author>
   </authors>
   <commentList>
-    <comment ref="F13" authorId="0">
+    <comment ref="F15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="68">
   <si>
     <t>recordedBy</t>
   </si>
@@ -245,6 +245,21 @@
   </si>
   <si>
     <t>date last changed</t>
+  </si>
+  <si>
+    <t>metadata</t>
+  </si>
+  <si>
+    <t>plate information</t>
+  </si>
+  <si>
+    <t>fileValue</t>
+  </si>
+  <si>
+    <t>source file</t>
+  </si>
+  <si>
+    <t>uploadedPlates/ABC.sdf</t>
   </si>
 </sst>
 </file>
@@ -306,8 +321,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="473">
+  <cellStyleXfs count="479">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -785,7 +806,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="473">
+  <cellStyles count="479">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1022,6 +1043,9 @@
     <cellStyle name="Followed Hyperlink" xfId="468" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="470" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="472" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="474" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="476" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="478" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1258,6 +1282,9 @@
     <cellStyle name="Hyperlink" xfId="467" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="469" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="471" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="473" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="475" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="477" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1587,11 +1614,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1742,46 +1769,46 @@
         <v>22</v>
       </c>
     </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" t="s">
+        <v>64</v>
+      </c>
+    </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>17</v>
       </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
       <c r="E10" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="F10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>0</v>
-      </c>
-      <c r="G11" t="s">
-        <v>12</v>
+        <v>66</v>
+      </c>
+      <c r="H10" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
       <c r="E12" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="F12" t="s">
-        <v>37</v>
-      </c>
-      <c r="G12" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1789,13 +1816,10 @@
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13" t="s">
-        <v>38</v>
+        <v>0</v>
+      </c>
+      <c r="G13" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1803,34 +1827,33 @@
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E14" t="s">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="F14" t="s">
-        <v>60</v>
-      </c>
-      <c r="H14" s="1"/>
+        <v>37</v>
+      </c>
+      <c r="G14" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>17</v>
       </c>
-      <c r="C15" t="s">
-        <v>7</v>
+      <c r="B15" t="s">
+        <v>6</v>
       </c>
       <c r="E15" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="F15" t="s">
-        <v>39</v>
-      </c>
-      <c r="G15" t="s">
-        <v>25</v>
-      </c>
-      <c r="H15" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1844,7 +1867,7 @@
         <v>59</v>
       </c>
       <c r="F16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H16" s="1"/>
     </row>
@@ -1856,47 +1879,48 @@
         <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F17" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="G17" t="s">
-        <v>56</v>
+        <v>25</v>
+      </c>
+      <c r="H17" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="C18" t="s">
-        <v>7</v>
+      <c r="B18" t="s">
+        <v>6</v>
       </c>
       <c r="E18" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="F18" t="s">
-        <v>40</v>
-      </c>
-      <c r="G18" t="s">
-        <v>41</v>
-      </c>
-      <c r="H18">
-        <v>10</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>17</v>
       </c>
-      <c r="D19" t="s">
-        <v>42</v>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" t="s">
+        <v>13</v>
       </c>
       <c r="G19" t="s">
-        <v>43</v>
-      </c>
-      <c r="H19" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1910,10 +1934,10 @@
         <v>16</v>
       </c>
       <c r="F20" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G20" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H20">
         <v>10</v>
@@ -1927,10 +1951,10 @@
         <v>42</v>
       </c>
       <c r="G21" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="H21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1941,49 +1965,61 @@
         <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="F22" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="G22" t="s">
-        <v>50</v>
-      </c>
-      <c r="H22" s="1">
-        <v>41218</v>
+        <v>47</v>
+      </c>
+      <c r="H22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" t="s">
+        <v>48</v>
+      </c>
+      <c r="H23" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>17</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="F24" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" t="s">
-        <v>0</v>
-      </c>
-      <c r="G25" t="s">
-        <v>12</v>
+        <v>62</v>
+      </c>
+      <c r="G24" t="s">
+        <v>50</v>
+      </c>
+      <c r="H24" s="1">
+        <v>41218</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>51</v>
       </c>
-      <c r="B26" t="s">
-        <v>52</v>
-      </c>
-      <c r="G26" t="s">
-        <v>55</v>
+      <c r="E26" t="s">
+        <v>58</v>
+      </c>
+      <c r="F26" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1991,9 +2027,31 @@
         <v>51</v>
       </c>
       <c r="B27" t="s">
+        <v>0</v>
+      </c>
+      <c r="G27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" t="s">
+        <v>52</v>
+      </c>
+      <c r="G28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" t="s">
         <v>54</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G29" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>